<commit_message>
Push code to branch chandy
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -446,44 +446,44 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Solin Neat</t>
+          <t>Chandy Neat</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-11-22</t>
+          <t>2024-11-25</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>20:50:27</t>
+          <t>07:39:25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2024-11-22 20:50:27</t>
+          <t>2024-11-25 07:39:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Chandy Neat</t>
+          <t>Koemthay Tha</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2024-11-22</t>
+          <t>2024-11-25</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>20:50:27</t>
+          <t>07:39:45</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2024-11-22 20:50:27</t>
+          <t>2024-11-25 07:39:45</t>
         </is>
       </c>
     </row>

</xml_diff>